<commit_message>
Padam Templates and TTD 03/01/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
@@ -3346,9 +3346,9 @@
   <dimension ref="A1:X1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1223" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N817" sqref="N817"/>
+      <selection pane="bottomLeft" activeCell="N152" sqref="N152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS 4.5 FINAL - PARAAA
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3221" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3220" uniqueCount="898">
   <si>
     <t>PS</t>
   </si>
@@ -2718,13 +2718,16 @@
   </si>
   <si>
     <t xml:space="preserve">iShu#mataq itIShu# - maqteq </t>
+  </si>
+  <si>
+    <t>NE + NRE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2847,6 +2850,12 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -3070,10 +3079,10 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3358,10 +3367,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1219" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A863" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1235" sqref="N1235"/>
+      <selection pane="bottomLeft" activeCell="X1064" sqref="X1064"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -45046,9 +45055,6 @@
       <c r="R1062" s="8"/>
       <c r="S1062" s="8"/>
       <c r="T1062" s="8"/>
-      <c r="U1062" s="64" t="s">
-        <v>821</v>
-      </c>
       <c r="V1062" s="8"/>
       <c r="W1062" s="8"/>
       <c r="X1062" s="51"/>
@@ -45084,7 +45090,9 @@
       <c r="R1063" s="8"/>
       <c r="S1063" s="8"/>
       <c r="T1063" s="8"/>
-      <c r="U1063" s="8"/>
+      <c r="U1063" s="64" t="s">
+        <v>897</v>
+      </c>
       <c r="V1063" s="8"/>
       <c r="W1063" s="8"/>
       <c r="X1063" s="51"/>
@@ -45120,9 +45128,7 @@
       <c r="R1064" s="8"/>
       <c r="S1064" s="8"/>
       <c r="T1064" s="8"/>
-      <c r="U1064" s="64" t="s">
-        <v>808</v>
-      </c>
+      <c r="U1064" s="8"/>
       <c r="V1064" s="8"/>
       <c r="W1064" s="8"/>
       <c r="X1064" s="51"/>

</xml_diff>

<commit_message>
TS 4.5 other edits SS
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3221" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3226" uniqueCount="897">
   <si>
     <t>PS</t>
   </si>
@@ -3383,10 +3383,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1235"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="L54" sqref="L54"/>
+      <selection pane="bottomLeft" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -25476,7 +25476,9 @@
       <c r="N541" s="17" t="s">
         <v>861</v>
       </c>
-      <c r="O541" s="3"/>
+      <c r="O541" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="P541" s="49"/>
       <c r="Q541" s="8"/>
       <c r="R541" s="8"/>
@@ -27313,7 +27315,9 @@
       <c r="N589" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="O589" s="3"/>
+      <c r="O589" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="P589" s="49"/>
       <c r="Q589" s="8"/>
       <c r="R589" s="8"/>
@@ -30472,7 +30476,9 @@
       <c r="N671" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="O671" s="1"/>
+      <c r="O671" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="P671" s="49"/>
       <c r="Q671" s="8"/>
       <c r="R671" s="8"/>
@@ -38755,6 +38761,9 @@
       <c r="N894" s="17" t="s">
         <v>857</v>
       </c>
+      <c r="O894" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="P894" s="49"/>
       <c r="Q894" s="8"/>
       <c r="R894" s="8"/>
@@ -43824,7 +43833,9 @@
       <c r="N1029" s="56" t="s">
         <v>832</v>
       </c>
-      <c r="O1029" s="1"/>
+      <c r="O1029" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="P1029" s="49"/>
       <c r="Q1029" s="8"/>
       <c r="R1029" s="8"/>

</xml_diff>

<commit_message>
TS 4.5 Temp,Raja files and Swaram ppt 25/01/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
@@ -3530,10 +3530,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="I582" sqref="I582"/>
+      <selection pane="bottomLeft" activeCell="N95" sqref="N95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
All edits of Templates, Chamakam for Raja 31/01/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3974" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4148" uniqueCount="926">
   <si>
     <t>PS</t>
   </si>
@@ -2811,13 +2811,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3026,212 +3032,215 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3515,10 +3524,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A393" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="R152" sqref="R152"/>
+      <selection pane="bottomLeft" activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6292,7 +6301,9 @@
       <c r="B52" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C52" s="9"/>
+      <c r="C52" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D52" s="29"/>
       <c r="E52" s="26"/>
       <c r="F52" s="26"/>
@@ -6331,6 +6342,9 @@
       <c r="B53" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C53" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D53" s="30"/>
       <c r="E53" s="25"/>
       <c r="F53" s="25"/>
@@ -6380,7 +6394,9 @@
       <c r="B54" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C54" s="9"/>
+      <c r="C54" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D54" s="29"/>
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
@@ -6421,7 +6437,9 @@
       <c r="B55" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C55" s="9"/>
+      <c r="C55" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D55" s="29"/>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
@@ -6466,7 +6484,9 @@
       <c r="B56" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C56" s="9"/>
+      <c r="C56" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D56" s="29"/>
       <c r="E56" s="26"/>
       <c r="F56" s="26"/>
@@ -6507,7 +6527,9 @@
       <c r="B57" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C57" s="9"/>
+      <c r="C57" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D57" s="29"/>
       <c r="E57" s="26"/>
       <c r="F57" s="26"/>
@@ -6548,7 +6570,9 @@
       <c r="B58" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C58" s="9"/>
+      <c r="C58" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D58" s="29"/>
       <c r="E58" s="26"/>
       <c r="F58" s="26"/>
@@ -6589,7 +6613,9 @@
       <c r="B59" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C59" s="9"/>
+      <c r="C59" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D59" s="29"/>
       <c r="E59" s="26"/>
       <c r="F59" s="26"/>
@@ -6630,7 +6656,9 @@
       <c r="B60" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C60" s="9"/>
+      <c r="C60" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D60" s="29"/>
       <c r="E60" s="26"/>
       <c r="F60" s="26"/>
@@ -6670,6 +6698,9 @@
       <c r="B61" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C61" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D61" s="30"/>
       <c r="E61" s="25"/>
       <c r="F61" s="25"/>
@@ -6715,6 +6746,9 @@
     <row r="62" spans="1:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C62" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="25"/>
@@ -6758,6 +6792,9 @@
       <c r="B63" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C63" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D63" s="30"/>
       <c r="E63" s="25"/>
       <c r="F63" s="25"/>
@@ -6801,7 +6838,9 @@
       <c r="B64" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C64" s="9"/>
+      <c r="C64" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D64" s="29"/>
       <c r="E64" s="26"/>
       <c r="F64" s="26"/>
@@ -6842,7 +6881,9 @@
       <c r="B65" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C65" s="9"/>
+      <c r="C65" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D65" s="29"/>
       <c r="E65" s="26"/>
       <c r="F65" s="26"/>
@@ -6883,7 +6924,9 @@
       <c r="B66" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C66" s="9"/>
+      <c r="C66" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D66" s="63" t="s">
         <v>884</v>
       </c>
@@ -6928,7 +6971,9 @@
       <c r="B67" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C67" s="9"/>
+      <c r="C67" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D67" s="29"/>
       <c r="E67" s="26"/>
       <c r="F67" s="26"/>
@@ -6973,7 +7018,9 @@
       <c r="B68" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C68" s="9"/>
+      <c r="C68" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D68" s="29"/>
       <c r="E68" s="26"/>
       <c r="F68" s="26"/>
@@ -7014,7 +7061,9 @@
       <c r="B69" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C69" s="9"/>
+      <c r="C69" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D69" s="29"/>
       <c r="E69" s="26"/>
       <c r="F69" s="26"/>
@@ -7055,7 +7104,9 @@
       <c r="B70" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C70" s="9"/>
+      <c r="C70" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D70" s="29"/>
       <c r="E70" s="26"/>
       <c r="F70" s="26"/>
@@ -7094,6 +7145,9 @@
     <row r="71" spans="1:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C71" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="25"/>
@@ -7137,6 +7191,9 @@
       <c r="B72" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C72" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D72" s="30"/>
       <c r="E72" s="25"/>
       <c r="F72" s="25"/>
@@ -7180,7 +7237,9 @@
       <c r="B73" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C73" s="9"/>
+      <c r="C73" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D73" s="29"/>
       <c r="E73" s="26"/>
       <c r="F73" s="26"/>
@@ -7220,6 +7279,9 @@
       <c r="B74" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C74" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D74" s="30"/>
       <c r="E74" s="25"/>
       <c r="F74" s="25"/>
@@ -7266,6 +7328,9 @@
       <c r="B75" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C75" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D75" s="30"/>
       <c r="E75" s="25"/>
       <c r="F75" s="25"/>
@@ -7313,7 +7378,9 @@
       <c r="B76" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C76" s="9"/>
+      <c r="C76" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D76" s="29"/>
       <c r="E76" s="26"/>
       <c r="F76" s="26"/>
@@ -7356,6 +7423,9 @@
     <row r="77" spans="1:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C77" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D77" s="30"/>
       <c r="E77" s="25"/>
@@ -7401,6 +7471,9 @@
       <c r="B78" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C78" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D78" s="30"/>
       <c r="E78" s="25"/>
       <c r="F78" s="25"/>
@@ -7451,7 +7524,9 @@
       <c r="B79" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C79" s="9"/>
+      <c r="C79" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D79" s="29"/>
       <c r="E79" s="26"/>
       <c r="F79" s="26"/>
@@ -7492,6 +7567,9 @@
     <row r="80" spans="1:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C80" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D80" s="30"/>
       <c r="E80" s="25"/>
@@ -7537,6 +7615,9 @@
       <c r="B81" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C81" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D81" s="30"/>
       <c r="E81" s="25"/>
       <c r="F81" s="25"/>
@@ -7583,6 +7664,9 @@
       <c r="B82" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C82" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D82" s="30"/>
       <c r="E82" s="25"/>
       <c r="F82" s="25"/>
@@ -7630,6 +7714,9 @@
     <row r="83" spans="1:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C83" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D83" s="30"/>
       <c r="E83" s="25"/>
@@ -7675,6 +7762,9 @@
       <c r="B84" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C84" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D84" s="30"/>
       <c r="E84" s="25"/>
       <c r="F84" s="25"/>
@@ -7722,6 +7812,9 @@
     <row r="85" spans="1:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C85" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D85" s="30"/>
       <c r="E85" s="25"/>
@@ -7767,6 +7860,9 @@
       <c r="B86" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C86" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D86" s="30"/>
       <c r="E86" s="25"/>
       <c r="F86" s="25"/>
@@ -7809,6 +7905,9 @@
       <c r="B87" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C87" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D87" s="30"/>
       <c r="E87" s="25"/>
       <c r="F87" s="25"/>
@@ -7851,6 +7950,9 @@
       <c r="B88" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C88" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D88" s="30"/>
       <c r="E88" s="25"/>
       <c r="F88" s="25"/>
@@ -7898,6 +8000,9 @@
     <row r="89" spans="1:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C89" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D89" s="30"/>
       <c r="E89" s="25"/>
@@ -7942,6 +8047,9 @@
     <row r="90" spans="1:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C90" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="25"/>
@@ -7986,7 +8094,9 @@
       <c r="B91" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C91" s="9"/>
+      <c r="C91" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D91" s="29"/>
       <c r="E91" s="26"/>
       <c r="F91" s="26"/>
@@ -8027,7 +8137,9 @@
       <c r="B92" s="68" t="s">
         <v>915</v>
       </c>
-      <c r="C92" s="9"/>
+      <c r="C92" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D92" s="29"/>
       <c r="E92" s="26"/>
       <c r="F92" s="26"/>
@@ -8068,6 +8180,9 @@
     <row r="93" spans="1:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C93" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D93" s="30"/>
       <c r="E93" s="25"/>
@@ -8111,6 +8226,9 @@
       <c r="B94" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C94" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D94" s="30"/>
       <c r="E94" s="25"/>
       <c r="F94" s="25"/>
@@ -8153,6 +8271,9 @@
       <c r="B95" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C95" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D95" s="30"/>
       <c r="E95" s="25"/>
       <c r="F95" s="25"/>
@@ -8200,6 +8321,9 @@
     <row r="96" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C96" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D96" s="30"/>
       <c r="E96" s="25"/>
@@ -8243,6 +8367,9 @@
       <c r="B97" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C97" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D97" s="30"/>
       <c r="E97" s="25"/>
       <c r="F97" s="25"/>
@@ -8285,6 +8412,9 @@
       <c r="B98" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C98" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D98" s="30"/>
       <c r="E98" s="25"/>
       <c r="F98" s="25"/>
@@ -8327,6 +8457,9 @@
       <c r="B99" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C99" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D99" s="30"/>
       <c r="E99" s="25"/>
       <c r="F99" s="25"/>
@@ -8369,6 +8502,9 @@
       <c r="B100" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C100" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D100" s="30"/>
       <c r="E100" s="25"/>
       <c r="F100" s="25"/>
@@ -8412,6 +8548,9 @@
     <row r="101" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C101" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D101" s="30"/>
       <c r="E101" s="25"/>
@@ -8455,6 +8594,9 @@
       <c r="B102" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C102" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D102" s="30"/>
       <c r="E102" s="25"/>
       <c r="F102" s="25"/>
@@ -8496,6 +8638,9 @@
       <c r="B103" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C103" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D103" s="30"/>
       <c r="E103" s="25"/>
       <c r="F103" s="25"/>
@@ -8541,6 +8686,9 @@
     <row r="104" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C104" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D104" s="30"/>
       <c r="E104" s="25"/>
@@ -8584,6 +8732,9 @@
       <c r="B105" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C105" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D105" s="30"/>
       <c r="E105" s="25"/>
       <c r="F105" s="25"/>
@@ -8626,6 +8777,9 @@
       <c r="B106" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C106" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D106" s="30"/>
       <c r="E106" s="25"/>
       <c r="F106" s="25"/>
@@ -8668,6 +8822,9 @@
       <c r="B107" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C107" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D107" s="30"/>
       <c r="E107" s="25"/>
       <c r="F107" s="25"/>
@@ -8713,6 +8870,9 @@
     <row r="108" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B108" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C108" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D108" s="30"/>
       <c r="E108" s="25"/>
@@ -8757,6 +8917,9 @@
     <row r="109" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C109" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D109" s="30"/>
       <c r="E109" s="25"/>
@@ -8800,6 +8963,9 @@
       <c r="B110" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C110" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D110" s="30"/>
       <c r="E110" s="25"/>
       <c r="F110" s="25"/>
@@ -8846,6 +9012,9 @@
       <c r="B111" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C111" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D111" s="30"/>
       <c r="E111" s="25"/>
       <c r="F111" s="25"/>
@@ -8892,6 +9061,9 @@
       <c r="B112" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C112" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D112" s="30"/>
       <c r="E112" s="25"/>
       <c r="F112" s="25"/>
@@ -8939,6 +9111,9 @@
     <row r="113" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C113" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D113" s="30"/>
       <c r="E113" s="25"/>
@@ -8982,6 +9157,9 @@
       <c r="B114" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C114" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D114" s="30"/>
       <c r="E114" s="25"/>
       <c r="F114" s="25"/>
@@ -9024,6 +9202,9 @@
       <c r="B115" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C115" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D115" s="30"/>
       <c r="E115" s="25"/>
       <c r="F115" s="25"/>
@@ -9071,6 +9252,9 @@
     <row r="116" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C116" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D116" s="30"/>
       <c r="E116" s="25"/>
@@ -9116,6 +9300,9 @@
       <c r="B117" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C117" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D117" s="30"/>
       <c r="E117" s="25"/>
       <c r="F117" s="25"/>
@@ -9162,6 +9349,9 @@
       <c r="B118" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C118" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D118" s="30"/>
       <c r="E118" s="25"/>
       <c r="F118" s="25"/>
@@ -9211,6 +9401,9 @@
     <row r="119" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C119" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D119" s="30"/>
       <c r="E119" s="25"/>
@@ -9254,6 +9447,9 @@
       <c r="B120" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C120" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D120" s="30"/>
       <c r="E120" s="25"/>
       <c r="F120" s="25"/>
@@ -9296,6 +9492,9 @@
       <c r="B121" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C121" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D121" s="30"/>
       <c r="E121" s="25"/>
       <c r="F121" s="25"/>
@@ -9338,6 +9537,9 @@
       <c r="B122" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C122" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D122" s="30"/>
       <c r="E122" s="25"/>
       <c r="F122" s="25"/>
@@ -9380,6 +9582,9 @@
       <c r="B123" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C123" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D123" s="30"/>
       <c r="E123" s="25"/>
       <c r="F123" s="25"/>
@@ -9422,6 +9627,9 @@
       <c r="B124" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C124" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D124" s="30"/>
       <c r="E124" s="25"/>
       <c r="F124" s="25"/>
@@ -9464,6 +9672,9 @@
       <c r="B125" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C125" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D125" s="30"/>
       <c r="E125" s="25"/>
       <c r="F125" s="25"/>
@@ -9506,6 +9717,9 @@
       <c r="B126" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C126" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D126" s="30"/>
       <c r="E126" s="25"/>
       <c r="F126" s="25"/>
@@ -9551,6 +9765,9 @@
     <row r="127" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C127" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D127" s="30"/>
       <c r="E127" s="25"/>
@@ -9594,6 +9811,9 @@
       <c r="B128" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C128" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D128" s="64" t="s">
         <v>883</v>
       </c>
@@ -9640,6 +9860,9 @@
       <c r="B129" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C129" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D129" s="30"/>
       <c r="E129" s="25"/>
       <c r="F129" s="25"/>
@@ -9686,6 +9909,9 @@
       <c r="B130" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C130" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D130" s="30"/>
       <c r="E130" s="25"/>
       <c r="F130" s="25"/>
@@ -9732,6 +9958,9 @@
       <c r="B131" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C131" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D131" s="30"/>
       <c r="E131" s="25"/>
       <c r="F131" s="25"/>
@@ -9778,9 +10007,14 @@
       <c r="B132" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C132" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D132" s="30"/>
       <c r="E132" s="25"/>
-      <c r="F132" s="25"/>
+      <c r="F132" s="78" t="s">
+        <v>913</v>
+      </c>
       <c r="G132" s="25"/>
       <c r="H132" s="67" t="s">
         <v>899</v>
@@ -9826,9 +10060,14 @@
       <c r="B133" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C133" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D133" s="30"/>
       <c r="E133" s="25"/>
-      <c r="F133" s="25"/>
+      <c r="F133" s="78" t="s">
+        <v>913</v>
+      </c>
       <c r="G133" s="25"/>
       <c r="H133" s="67" t="s">
         <v>899</v>
@@ -9870,6 +10109,9 @@
       <c r="B134" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C134" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D134" s="30"/>
       <c r="E134" s="25"/>
       <c r="F134" s="25"/>
@@ -9915,6 +10157,9 @@
     <row r="135" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B135" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C135" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D135" s="30"/>
       <c r="E135" s="25"/>
@@ -9960,6 +10205,9 @@
       <c r="B136" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C136" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D136" s="30"/>
       <c r="E136" s="25"/>
       <c r="F136" s="25"/>
@@ -10004,6 +10252,9 @@
       <c r="B137" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C137" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D137" s="30"/>
       <c r="E137" s="25"/>
       <c r="F137" s="25"/>
@@ -10048,6 +10299,9 @@
       <c r="B138" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C138" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D138" s="64" t="s">
         <v>887</v>
       </c>
@@ -10094,6 +10348,9 @@
       <c r="B139" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C139" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D139" s="30"/>
       <c r="E139" s="25"/>
       <c r="F139" s="25"/>
@@ -10139,6 +10396,9 @@
     <row r="140" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B140" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C140" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D140" s="30"/>
       <c r="E140" s="25"/>
@@ -10183,6 +10443,9 @@
     <row r="141" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B141" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C141" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D141" s="30"/>
       <c r="E141" s="25"/>
@@ -10226,6 +10489,9 @@
       <c r="B142" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C142" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D142" s="30"/>
       <c r="E142" s="25"/>
       <c r="F142" s="25"/>
@@ -10268,6 +10534,9 @@
       <c r="B143" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C143" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D143" s="30"/>
       <c r="E143" s="25"/>
       <c r="F143" s="25"/>
@@ -10310,6 +10579,9 @@
       <c r="B144" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C144" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D144" s="30"/>
       <c r="E144" s="25"/>
       <c r="F144" s="25"/>
@@ -10352,6 +10624,9 @@
       <c r="B145" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C145" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D145" s="30"/>
       <c r="E145" s="25"/>
       <c r="F145" s="25"/>
@@ -10394,6 +10669,9 @@
       <c r="B146" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C146" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D146" s="30"/>
       <c r="E146" s="25"/>
       <c r="F146" s="25"/>
@@ -10439,6 +10717,9 @@
     <row r="147" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C147" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D147" s="30"/>
       <c r="E147" s="25"/>
@@ -10482,6 +10763,9 @@
       <c r="B148" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C148" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D148" s="30"/>
       <c r="E148" s="25"/>
       <c r="F148" s="25"/>
@@ -10524,6 +10808,9 @@
       <c r="B149" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C149" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D149" s="30"/>
       <c r="E149" s="25"/>
       <c r="F149" s="25"/>
@@ -10566,6 +10853,9 @@
       <c r="B150" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C150" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D150" s="30"/>
       <c r="E150" s="25"/>
       <c r="F150" s="25"/>
@@ -10608,6 +10898,9 @@
       <c r="B151" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C151" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D151" s="30"/>
       <c r="E151" s="25"/>
       <c r="F151" s="25"/>
@@ -10650,6 +10943,9 @@
       <c r="B152" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C152" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D152" s="30"/>
       <c r="E152" s="25"/>
       <c r="F152" s="25"/>
@@ -10692,6 +10988,9 @@
     <row r="153" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B153" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C153" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D153" s="30"/>
       <c r="E153" s="25"/>
@@ -10735,6 +11034,9 @@
       <c r="B154" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C154" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D154" s="30"/>
       <c r="E154" s="25"/>
       <c r="F154" s="25"/>
@@ -10781,6 +11083,9 @@
       <c r="B155" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C155" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D155" s="30"/>
       <c r="E155" s="25"/>
       <c r="F155" s="25"/>
@@ -10826,6 +11131,9 @@
     <row r="156" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B156" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C156" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D156" s="30"/>
       <c r="E156" s="25"/>
@@ -10872,6 +11180,9 @@
     <row r="157" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B157" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C157" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D157" s="30"/>
       <c r="E157" s="25"/>
@@ -10915,6 +11226,9 @@
       <c r="B158" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C158" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D158" s="30"/>
       <c r="E158" s="25"/>
       <c r="F158" s="25"/>
@@ -10957,6 +11271,9 @@
       <c r="B159" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C159" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D159" s="30"/>
       <c r="E159" s="25"/>
       <c r="F159" s="25"/>
@@ -11003,6 +11320,9 @@
       <c r="B160" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C160" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D160" s="30"/>
       <c r="E160" s="25"/>
       <c r="F160" s="25"/>
@@ -11050,6 +11370,9 @@
     <row r="161" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B161" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C161" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D161" s="30"/>
       <c r="E161" s="25"/>
@@ -11096,6 +11419,9 @@
     <row r="162" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B162" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C162" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D162" s="30"/>
       <c r="E162" s="25"/>
@@ -11139,6 +11465,9 @@
       <c r="B163" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C163" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D163" s="30"/>
       <c r="E163" s="25"/>
       <c r="F163" s="25"/>
@@ -11181,6 +11510,9 @@
       <c r="B164" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C164" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D164" s="30"/>
       <c r="E164" s="25"/>
       <c r="F164" s="25"/>
@@ -11223,6 +11555,9 @@
       <c r="B165" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C165" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D165" s="30"/>
       <c r="E165" s="25"/>
       <c r="F165" s="25"/>
@@ -11265,6 +11600,9 @@
       <c r="B166" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C166" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D166" s="30"/>
       <c r="E166" s="25"/>
       <c r="F166" s="25"/>
@@ -11311,6 +11649,9 @@
       <c r="B167" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C167" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D167" s="30"/>
       <c r="E167" s="25"/>
       <c r="F167" s="25"/>
@@ -11356,6 +11697,9 @@
     <row r="168" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B168" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C168" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D168" s="30"/>
       <c r="E168" s="25"/>
@@ -11402,6 +11746,9 @@
     <row r="169" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B169" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C169" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D169" s="30"/>
       <c r="E169" s="25"/>
@@ -11445,6 +11792,9 @@
       <c r="B170" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C170" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D170" s="30"/>
       <c r="E170" s="25"/>
       <c r="F170" s="25"/>
@@ -11487,6 +11837,9 @@
       <c r="B171" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C171" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D171" s="30"/>
       <c r="E171" s="25"/>
       <c r="F171" s="25"/>
@@ -11533,6 +11886,9 @@
       <c r="B172" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C172" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D172" s="64" t="s">
         <v>885</v>
       </c>
@@ -11584,6 +11940,9 @@
     <row r="173" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B173" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C173" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D173" s="30"/>
       <c r="E173" s="25"/>
@@ -11630,6 +11989,9 @@
     <row r="174" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B174" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C174" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D174" s="30"/>
       <c r="E174" s="25"/>
@@ -11675,6 +12037,9 @@
       <c r="B175" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C175" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D175" s="30"/>
       <c r="E175" s="25"/>
       <c r="F175" s="25"/>
@@ -11720,6 +12085,9 @@
     <row r="176" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B176" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C176" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D176" s="30"/>
       <c r="E176" s="25"/>
@@ -11765,6 +12133,9 @@
       <c r="B177" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C177" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D177" s="30"/>
       <c r="E177" s="25"/>
       <c r="F177" s="25"/>
@@ -11809,6 +12180,9 @@
       <c r="B178" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C178" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D178" s="30"/>
       <c r="E178" s="25"/>
       <c r="F178" s="25"/>
@@ -11853,6 +12227,9 @@
       <c r="B179" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C179" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D179" s="30"/>
       <c r="E179" s="25"/>
       <c r="F179" s="25"/>
@@ -11902,6 +12279,9 @@
     <row r="180" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B180" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C180" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D180" s="30"/>
       <c r="E180" s="25"/>
@@ -11945,6 +12325,9 @@
       <c r="B181" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C181" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D181" s="30"/>
       <c r="E181" s="25"/>
       <c r="F181" s="25"/>
@@ -11987,6 +12370,9 @@
       <c r="B182" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C182" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D182" s="30"/>
       <c r="E182" s="25"/>
       <c r="F182" s="25"/>
@@ -12029,6 +12415,9 @@
       <c r="B183" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C183" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D183" s="30"/>
       <c r="E183" s="25"/>
       <c r="F183" s="25"/>
@@ -12074,6 +12463,9 @@
     <row r="184" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B184" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C184" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D184" s="30"/>
       <c r="E184" s="25"/>
@@ -12117,6 +12509,9 @@
       <c r="B185" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C185" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D185" s="30"/>
       <c r="E185" s="25"/>
       <c r="F185" s="25"/>
@@ -12159,6 +12554,9 @@
       <c r="B186" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C186" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D186" s="30"/>
       <c r="E186" s="25"/>
       <c r="F186" s="25"/>
@@ -12201,6 +12599,9 @@
       <c r="B187" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C187" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D187" s="30"/>
       <c r="E187" s="25"/>
       <c r="F187" s="25"/>
@@ -12246,6 +12647,9 @@
     <row r="188" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B188" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C188" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D188" s="30"/>
       <c r="E188" s="25"/>
@@ -12289,6 +12693,9 @@
       <c r="B189" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C189" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D189" s="30"/>
       <c r="E189" s="25"/>
       <c r="F189" s="25"/>
@@ -12332,6 +12739,9 @@
     <row r="190" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B190" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C190" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D190" s="30"/>
       <c r="E190" s="25"/>
@@ -12375,6 +12785,9 @@
       <c r="B191" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C191" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D191" s="30"/>
       <c r="E191" s="25"/>
       <c r="F191" s="25"/>
@@ -12417,6 +12830,9 @@
       <c r="B192" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C192" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D192" s="30"/>
       <c r="E192" s="25"/>
       <c r="F192" s="25"/>
@@ -12459,6 +12875,9 @@
       <c r="B193" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C193" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D193" s="30"/>
       <c r="E193" s="25"/>
       <c r="F193" s="25"/>
@@ -12507,6 +12926,9 @@
       <c r="B194" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C194" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D194" s="30"/>
       <c r="E194" s="25"/>
       <c r="F194" s="25"/>
@@ -12552,6 +12974,9 @@
     <row r="195" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B195" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C195" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D195" s="30"/>
       <c r="E195" s="25"/>
@@ -12597,6 +13022,9 @@
       <c r="B196" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C196" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D196" s="30"/>
       <c r="E196" s="25"/>
       <c r="F196" s="25"/>
@@ -12641,6 +13069,9 @@
       <c r="B197" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C197" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D197" s="64" t="s">
         <v>883</v>
       </c>
@@ -12688,6 +13119,9 @@
     <row r="198" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B198" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C198" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D198" s="30"/>
       <c r="E198" s="25"/>
@@ -12733,6 +13167,9 @@
       <c r="B199" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C199" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D199" s="30"/>
       <c r="E199" s="25"/>
       <c r="F199" s="25"/>
@@ -12781,6 +13218,9 @@
       <c r="B200" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C200" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D200" s="30"/>
       <c r="E200" s="25"/>
       <c r="F200" s="25"/>
@@ -12828,6 +13268,9 @@
     <row r="201" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B201" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C201" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D201" s="30"/>
       <c r="E201" s="25"/>
@@ -12871,6 +13314,9 @@
       <c r="B202" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C202" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D202" s="30"/>
       <c r="E202" s="25"/>
       <c r="F202" s="25"/>
@@ -12913,6 +13359,9 @@
       <c r="B203" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C203" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D203" s="30"/>
       <c r="E203" s="25"/>
       <c r="F203" s="25"/>
@@ -12955,6 +13404,9 @@
       <c r="B204" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C204" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D204" s="30"/>
       <c r="E204" s="25"/>
       <c r="F204" s="25"/>
@@ -12997,6 +13449,9 @@
       <c r="B205" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C205" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D205" s="30"/>
       <c r="E205" s="25"/>
       <c r="F205" s="25"/>
@@ -13042,6 +13497,9 @@
     <row r="206" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B206" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C206" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D206" s="30"/>
       <c r="E206" s="25"/>
@@ -13085,6 +13543,9 @@
       <c r="B207" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C207" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D207" s="30"/>
       <c r="E207" s="25"/>
       <c r="F207" s="25"/>
@@ -13130,6 +13591,9 @@
     <row r="208" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B208" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C208" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D208" s="30"/>
       <c r="E208" s="25"/>
@@ -13173,6 +13637,9 @@
     <row r="209" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B209" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C209" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D209" s="30"/>
       <c r="E209" s="25"/>
@@ -13216,6 +13683,9 @@
       <c r="B210" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C210" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D210" s="30"/>
       <c r="E210" s="25"/>
       <c r="F210" s="25"/>
@@ -13258,6 +13728,9 @@
       <c r="B211" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C211" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D211" s="30"/>
       <c r="E211" s="25"/>
       <c r="F211" s="25"/>
@@ -13300,6 +13773,9 @@
       <c r="B212" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C212" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D212" s="30"/>
       <c r="E212" s="25"/>
       <c r="F212" s="25"/>
@@ -13342,6 +13818,9 @@
       <c r="B213" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C213" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D213" s="30"/>
       <c r="E213" s="25"/>
       <c r="F213" s="25"/>
@@ -13384,6 +13863,9 @@
       <c r="B214" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C214" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D214" s="30"/>
       <c r="E214" s="25"/>
       <c r="F214" s="25"/>
@@ -13429,6 +13911,9 @@
     <row r="215" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B215" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C215" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D215" s="30"/>
       <c r="E215" s="25"/>
@@ -13481,6 +13966,9 @@
     <row r="216" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B216" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C216" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D216" s="30"/>
       <c r="E216" s="25"/>
@@ -13530,6 +14018,9 @@
       <c r="B217" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C217" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D217" s="30"/>
       <c r="E217" s="25"/>
       <c r="F217" s="25"/>
@@ -13577,6 +14068,9 @@
     <row r="218" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B218" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C218" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D218" s="30"/>
       <c r="E218" s="25"/>
@@ -13622,6 +14116,9 @@
       <c r="B219" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C219" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D219" s="30"/>
       <c r="E219" s="25"/>
       <c r="F219" s="25"/>
@@ -13666,6 +14163,9 @@
       <c r="B220" s="68" t="s">
         <v>915</v>
       </c>
+      <c r="C220" s="66" t="s">
+        <v>893</v>
+      </c>
       <c r="D220" s="30"/>
       <c r="E220" s="25"/>
       <c r="F220" s="25"/>
@@ -13709,6 +14209,9 @@
     <row r="221" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B221" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C221" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D221" s="30"/>
       <c r="E221" s="25"/>
@@ -13753,6 +14256,9 @@
     <row r="222" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B222" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C222" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D222" s="30"/>
       <c r="E222" s="25"/>
@@ -13795,6 +14301,9 @@
     <row r="223" spans="2:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B223" s="68" t="s">
         <v>915</v>
+      </c>
+      <c r="C223" s="66" t="s">
+        <v>893</v>
       </c>
       <c r="D223" s="30"/>
       <c r="E223" s="25"/>

</xml_diff>

<commit_message>
CG sanskrit 18022021 maamaa
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 4.5 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\Padam Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81D9AC9-9382-46DA-92F4-1D04C004A746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195E883C-F2D0-4AEF-9DED-82FD1D08B1AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3525,10 +3525,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomLeft" activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>